<commit_message>
Implementacion de cocktail sort junto a sus tiempos y grafica en exel
</commit_message>
<xml_diff>
--- a/AlgoritmosOrdenamiento/Libro1.xlsx
+++ b/AlgoritmosOrdenamiento/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angel Josue Loayza Huarachi_UCSP\Semestre 5 - 2022 - CCOMP5\ADA ♥♥♥\Algoritmos\AlgoritmosOrdenamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88D85E71-BC45-4994-B25C-302FFA4AC91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B66D7F-18F0-4ECA-A7FF-3F6069965081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8787BE03-EEF4-490F-871C-DE89A8461F90}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>n=1000</t>
   </si>
@@ -44,13 +44,16 @@
     <t>n=100</t>
   </si>
   <si>
-    <t>Booble sort</t>
-  </si>
-  <si>
     <t>Insert sort</t>
   </si>
   <si>
     <t>Select sort</t>
+  </si>
+  <si>
+    <t>Cocktail Sort</t>
+  </si>
+  <si>
+    <t>bubble sort</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Booble sort</c:v>
+                  <c:v>bubble sort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -417,6 +420,82 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1229-40CD-8334-66761B154238}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cocktail Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$J$4:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>n=100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>n=1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>n=10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$N$4:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D6F3-459F-907B-A5D9002F8E50}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1501,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A5184A-69FF-432C-9857-EC9D06138B82}">
-  <dimension ref="J3:M6"/>
+  <dimension ref="J3:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,18 +1594,21 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="10:14" x14ac:dyDescent="0.3">
       <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" t="s">
         <v>3</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>4</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
         <v>2</v>
       </c>
@@ -1539,8 +1621,11 @@
       <c r="M4">
         <v>1.2E-2</v>
       </c>
+      <c r="N4">
+        <v>8.9999999999999993E-3</v>
+      </c>
     </row>
-    <row r="5" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
         <v>0</v>
       </c>
@@ -1553,8 +1638,11 @@
       <c r="M5">
         <v>0.158</v>
       </c>
+      <c r="N5">
+        <v>7.0300000000000001E-2</v>
+      </c>
     </row>
-    <row r="6" spans="10:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J6" t="s">
         <v>1</v>
       </c>
@@ -1566,6 +1654,9 @@
       </c>
       <c r="M6">
         <v>0.30499999999999999</v>
+      </c>
+      <c r="N6">
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementacion de 3 nuevos algorimos, junto a un header.h de los algoritmos originales
</commit_message>
<xml_diff>
--- a/AlgoritmosOrdenamiento/Libro1.xlsx
+++ b/AlgoritmosOrdenamiento/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Angel Josue Loayza Huarachi_UCSP\Semestre 5 - 2022 - CCOMP5\ADA ♥♥♥\Algoritmos\AlgoritmosOrdenamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B66D7F-18F0-4ECA-A7FF-3F6069965081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1E906C-E24C-42D8-893C-AFEF22044BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8787BE03-EEF4-490F-871C-DE89A8461F90}"/>
   </bookViews>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>n=1000</t>
-  </si>
-  <si>
-    <t>n=10000</t>
   </si>
   <si>
     <t>n=100</t>
@@ -54,6 +51,18 @@
   </si>
   <si>
     <t>bubble sort</t>
+  </si>
+  <si>
+    <t>n=2000</t>
+  </si>
+  <si>
+    <t>Merge Sort</t>
+  </si>
+  <si>
+    <t>Quick Sort</t>
+  </si>
+  <si>
+    <t>Heap Sort</t>
   </si>
 </sst>
 </file>
@@ -245,7 +254,7 @@
                   <c:v>n=1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>n=10000</c:v>
+                  <c:v>n=2000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -257,13 +266,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0999999999999999E-2</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13500000000000001</c:v>
+                  <c:v>0.23100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32700000000000001</c:v>
+                  <c:v>0.41799999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -319,7 +328,7 @@
                   <c:v>n=1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>n=10000</c:v>
+                  <c:v>n=2000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -331,13 +340,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>2.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38200000000000001</c:v>
+                  <c:v>0.45400000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -393,7 +402,7 @@
                   <c:v>n=1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>n=10000</c:v>
+                  <c:v>n=2000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -405,13 +414,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.158</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30499999999999999</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -469,7 +478,7 @@
                   <c:v>n=1000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>n=10000</c:v>
+                  <c:v>n=2000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -481,13 +490,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0300000000000001E-2</c:v>
+                  <c:v>0.24399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,6 +505,235 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-D6F3-459F-907B-A5D9002F8E50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$J$4:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>n=100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>n=1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>n=2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$O$4:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40400000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2362-4F0A-AAEE-E5502BB25FB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$J$4:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>n=100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>n=1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>n=2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$P$4:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2362-4F0A-AAEE-E5502BB25FB8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heap Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$J$4:$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>n=100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>n=1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>n=2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$Q$4:$Q$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49099999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2362-4F0A-AAEE-E5502BB25FB8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1253,9 +1491,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>519430</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>815340</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1580,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A5184A-69FF-432C-9857-EC9D06138B82}">
-  <dimension ref="J3:N6"/>
+  <dimension ref="J3:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,69 +1832,105 @@
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="10:17" x14ac:dyDescent="0.3">
       <c r="K3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
-        <v>5</v>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1.0999999999999999E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="L4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="M4">
+        <v>0.02</v>
+      </c>
+      <c r="N4">
+        <v>0.02</v>
+      </c>
+      <c r="O4">
         <v>1.4E-2</v>
       </c>
-      <c r="M4">
-        <v>1.2E-2</v>
-      </c>
-      <c r="N4">
-        <v>8.9999999999999993E-3</v>
+      <c r="P4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="Q4">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J5" t="s">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0.13500000000000001</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="L5">
-        <v>0.15</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="M5">
-        <v>0.158</v>
+        <v>0.3</v>
       </c>
       <c r="N5">
-        <v>7.0300000000000001E-2</v>
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="O5">
+        <v>0.222</v>
+      </c>
+      <c r="P5">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="6" spans="10:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>0.32700000000000001</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="L6">
-        <v>0.38200000000000001</v>
+        <v>0.45400000000000001</v>
       </c>
       <c r="M6">
-        <v>0.30499999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="N6">
-        <v>0.22</v>
+        <v>0.6</v>
+      </c>
+      <c r="O6">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="P6">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="Q6">
+        <v>0.49099999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>